<commit_message>
adding wighted average calculation
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="22200" windowHeight="10335" tabRatio="804" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="22200" windowHeight="10335" tabRatio="804" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CITIES" sheetId="1" r:id="rId1"/>
     <sheet name="SCENARIOS" sheetId="2" r:id="rId2"/>
     <sheet name="FLOOR_AREA" sheetId="3" r:id="rId3"/>
+    <sheet name="FLOOR_AREA_CLIMATE" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CITIES!$A$2:$C$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CITIES!$A$1:$E$48</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="160">
   <si>
     <t>Albuquerque, NM</t>
   </si>
@@ -479,18 +480,49 @@
   </si>
   <si>
     <t>Extrapolation from past survey (coomercial 2003, 1999, residential 2009), sd maintained of latest survey</t>
+  </si>
+  <si>
+    <t>Very cold/Cold</t>
+  </si>
+  <si>
+    <t>Mixed-humid</t>
+  </si>
+  <si>
+    <t>Mixed-dry/Hot-dry</t>
+  </si>
+  <si>
+    <t>Hot-humid</t>
+  </si>
+  <si>
+    <t>Marine</t>
+  </si>
+  <si>
+    <t>GFA_mean_Commercial_perc</t>
+  </si>
+  <si>
+    <t>GFA_mean_Residential_perc</t>
+  </si>
+  <si>
+    <t>GFA_mean_Commercial_Miosqft</t>
+  </si>
+  <si>
+    <t>GFA_mean_Residential_Miosqft</t>
+  </si>
+  <si>
+    <t>Climate Region</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,6 +542,36 @@
       <color theme="1"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -519,7 +581,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -566,12 +628,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFont="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -592,10 +700,46 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Body: normal cell" xfId="2"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Parent row" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -873,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,9 +1028,10 @@
     <col min="1" max="1" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>107</v>
       </c>
@@ -899,53 +1044,65 @@
       <c r="D1" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="22" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C48" si="0">RIGHT(A2,LEN(A2)-SEARCH(",",A2,1))</f>
-        <v xml:space="preserve"> AK</v>
+        <f>RIGHT(A2,LEN(A2)-SEARCH(",",A2,1))</f>
+        <v xml:space="preserve"> HI</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> AL</v>
+        <f>RIGHT(A3,LEN(A3)-SEARCH(",",A3,1))</f>
+        <v xml:space="preserve"> FL</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> AR</v>
+        <f>RIGHT(A4,LEN(A4)-SEARCH(",",A4,1))</f>
+        <v xml:space="preserve"> TX</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
@@ -953,464 +1110,557 @@
         <v>67</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f>RIGHT(A5,LEN(A5)-SEARCH(",",A5,1))</f>
         <v xml:space="preserve"> AZ</v>
       </c>
       <c r="D5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="str">
+        <f>RIGHT(A6,LEN(A6)-SEARCH(",",A6,1))</f>
+        <v xml:space="preserve"> AL</v>
+      </c>
+      <c r="D6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="str">
+        <f>RIGHT(A7,LEN(A7)-SEARCH(",",A7,1))</f>
+        <v xml:space="preserve"> AR</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="str">
+        <f>RIGHT(A8,LEN(A8)-SEARCH(",",A8,1))</f>
+        <v xml:space="preserve"> GA</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="str">
+        <f>RIGHT(A9,LEN(A9)-SEARCH(",",A9,1))</f>
+        <v xml:space="preserve"> MS</v>
+      </c>
+      <c r="D9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="str">
+        <f>RIGHT(A10,LEN(A10)-SEARCH(",",A10,1))</f>
+        <v xml:space="preserve"> OK</v>
+      </c>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" t="str">
+        <f>RIGHT(A11,LEN(A11)-SEARCH(",",A11,1))</f>
+        <v xml:space="preserve"> SC</v>
+      </c>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B12" t="s">
         <v>69</v>
       </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
+      <c r="C12" t="str">
+        <f>RIGHT(A12,LEN(A12)-SEARCH(",",A12,1))</f>
         <v xml:space="preserve"> CA</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> CO</v>
-      </c>
-      <c r="D7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> CT</v>
-      </c>
-      <c r="D8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="E12" s="20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
+      <c r="C13" t="str">
+        <f>RIGHT(A13,LEN(A13)-SEARCH(",",A13,1))</f>
         <v xml:space="preserve"> DC</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D13" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="E13" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B14" t="s">
         <v>71</v>
       </c>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
+      <c r="C14" t="str">
+        <f>RIGHT(A14,LEN(A14)-SEARCH(",",A14,1))</f>
         <v xml:space="preserve"> DE</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D14" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> FL</v>
-      </c>
-      <c r="D11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> GA</v>
-      </c>
-      <c r="D12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> HI</v>
-      </c>
-      <c r="D13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> IA</v>
-      </c>
-      <c r="D14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> ID</v>
+        <f>RIGHT(A15,LEN(A15)-SEARCH(",",A15,1))</f>
+        <v xml:space="preserve"> KS</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> IL</v>
+        <f>RIGHT(A16,LEN(A16)-SEARCH(",",A16,1))</f>
+        <v xml:space="preserve"> KY</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> IN</v>
+        <f>RIGHT(A17,LEN(A17)-SEARCH(",",A17,1))</f>
+        <v xml:space="preserve"> MO</v>
       </c>
       <c r="D17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> KS</v>
+        <f>RIGHT(A18,LEN(A18)-SEARCH(",",A18,1))</f>
+        <v xml:space="preserve"> NC</v>
       </c>
       <c r="D18" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> KY</v>
+        <f>RIGHT(A19,LEN(A19)-SEARCH(",",A19,1))</f>
+        <v xml:space="preserve"> NY</v>
       </c>
       <c r="D19" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> MA</v>
+        <f>RIGHT(A20,LEN(A20)-SEARCH(",",A20,1))</f>
+        <v xml:space="preserve"> PA</v>
       </c>
       <c r="D20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="str">
+        <f>RIGHT(A21,LEN(A21)-SEARCH(",",A21,1))</f>
+        <v xml:space="preserve"> TN</v>
+      </c>
+      <c r="D21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" t="str">
+        <f>RIGHT(A22,LEN(A22)-SEARCH(",",A22,1))</f>
+        <v xml:space="preserve"> VA</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" t="str">
+        <f>RIGHT(A23,LEN(A23)-SEARCH(",",A23,1))</f>
+        <v xml:space="preserve"> WV</v>
+      </c>
+      <c r="D23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="str">
+        <f>RIGHT(A24,LEN(A24)-SEARCH(",",A24,1))</f>
+        <v xml:space="preserve"> NM</v>
+      </c>
+      <c r="D24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="str">
+        <f>RIGHT(A25,LEN(A25)-SEARCH(",",A25,1))</f>
+        <v xml:space="preserve"> OR</v>
+      </c>
+      <c r="D25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="str">
+        <f>RIGHT(A26,LEN(A26)-SEARCH(",",A26,1))</f>
+        <v xml:space="preserve"> WA</v>
+      </c>
+      <c r="D26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="str">
+        <f>RIGHT(A27,LEN(A27)-SEARCH(",",A27,1))</f>
+        <v xml:space="preserve"> CT</v>
+      </c>
+      <c r="D27" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> ME</v>
-      </c>
-      <c r="D21" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> MI</v>
-      </c>
-      <c r="D22" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> MN</v>
-      </c>
-      <c r="D23" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> MO</v>
-      </c>
-      <c r="D24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> MS</v>
-      </c>
-      <c r="D25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> NC</v>
-      </c>
-      <c r="D26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> ND</v>
-      </c>
-      <c r="D27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> NE</v>
+        <f>RIGHT(A28,LEN(A28)-SEARCH(",",A28,1))</f>
+        <v xml:space="preserve"> IA</v>
       </c>
       <c r="D28" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> NH</v>
+        <f>RIGHT(A29,LEN(A29)-SEARCH(",",A29,1))</f>
+        <v xml:space="preserve"> IL</v>
       </c>
       <c r="D29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> NJ</v>
+        <f>RIGHT(A30,LEN(A30)-SEARCH(",",A30,1))</f>
+        <v xml:space="preserve"> IN</v>
       </c>
       <c r="D30" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> NM</v>
+        <f>RIGHT(A31,LEN(A31)-SEARCH(",",A31,1))</f>
+        <v xml:space="preserve"> MA</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C32" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> NY</v>
+        <f>RIGHT(A32,LEN(A32)-SEARCH(",",A32,1))</f>
+        <v xml:space="preserve"> MI</v>
       </c>
       <c r="D32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="C33" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> OH</v>
+        <f>RIGHT(A33,LEN(A33)-SEARCH(",",A33,1))</f>
+        <v xml:space="preserve"> NE</v>
       </c>
       <c r="D33" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> OK</v>
+        <f>RIGHT(A34,LEN(A34)-SEARCH(",",A34,1))</f>
+        <v xml:space="preserve"> NJ</v>
       </c>
       <c r="D34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C35" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> OR</v>
+        <f>RIGHT(A35,LEN(A35)-SEARCH(",",A35,1))</f>
+        <v xml:space="preserve"> OH</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>32</v>
       </c>
@@ -1418,149 +1668,179 @@
         <v>86</v>
       </c>
       <c r="C36" t="str">
-        <f t="shared" si="0"/>
+        <f>RIGHT(A36,LEN(A36)-SEARCH(",",A36,1))</f>
         <v xml:space="preserve"> PA</v>
       </c>
       <c r="D36" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="C37" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> PA</v>
+        <f>RIGHT(A37,LEN(A37)-SEARCH(",",A37,1))</f>
+        <v xml:space="preserve"> RI</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="C38" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> RI</v>
+        <f>RIGHT(A38,LEN(A38)-SEARCH(",",A38,1))</f>
+        <v xml:space="preserve"> CO</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C39" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> SC</v>
+        <f>RIGHT(A39,LEN(A39)-SEARCH(",",A39,1))</f>
+        <v xml:space="preserve"> ID</v>
       </c>
       <c r="D39" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C40" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> TN</v>
+        <f>RIGHT(A40,LEN(A40)-SEARCH(",",A40,1))</f>
+        <v xml:space="preserve"> UT</v>
       </c>
       <c r="D40" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> TX</v>
+        <f>RIGHT(A41,LEN(A41)-SEARCH(",",A41,1))</f>
+        <v xml:space="preserve"> ME</v>
       </c>
       <c r="D41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> UT</v>
+        <f>RIGHT(A42,LEN(A42)-SEARCH(",",A42,1))</f>
+        <v xml:space="preserve"> MN</v>
       </c>
       <c r="D42" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> VA</v>
+        <f>RIGHT(A43,LEN(A43)-SEARCH(",",A43,1))</f>
+        <v xml:space="preserve"> ND</v>
       </c>
       <c r="D43" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> VT</v>
+        <f>RIGHT(A44,LEN(A44)-SEARCH(",",A44,1))</f>
+        <v xml:space="preserve"> NH</v>
       </c>
       <c r="D44" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> WA</v>
+        <f>RIGHT(A45,LEN(A45)-SEARCH(",",A45,1))</f>
+        <v xml:space="preserve"> VT</v>
       </c>
       <c r="D45" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>40</v>
       </c>
@@ -1568,48 +1848,63 @@
         <v>60</v>
       </c>
       <c r="C46" t="str">
-        <f t="shared" si="0"/>
+        <f>RIGHT(A46,LEN(A46)-SEARCH(",",A46,1))</f>
         <v xml:space="preserve"> WI</v>
       </c>
       <c r="D46" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> WV</v>
+        <f>RIGHT(A47,LEN(A47)-SEARCH(",",A47,1))</f>
+        <v xml:space="preserve"> WY</v>
       </c>
       <c r="D47" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> WY</v>
+        <f>RIGHT(A48,LEN(A48)-SEARCH(",",A48,1))</f>
+        <v xml:space="preserve"> AK</v>
       </c>
       <c r="D48" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E48">
+    <sortState ref="A2:E48">
+      <sortCondition ref="D1:D48"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A1:C81">
     <sortCondition ref="C1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1794,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,4 +2365,157 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="115.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="14">
+        <v>31898</v>
+      </c>
+      <c r="C2" s="15">
+        <f>B2/SUM(B$2:B$6)</f>
+        <v>0.36625216722354265</v>
+      </c>
+      <c r="D2" s="19">
+        <v>42.5</v>
+      </c>
+      <c r="E2" s="18">
+        <f>D2/SUM(D$2:D$6)</f>
+        <v>0.35956006768189508</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="14">
+        <v>27873</v>
+      </c>
+      <c r="C3" s="15">
+        <f t="shared" ref="C3:E6" si="0">B3/SUM(B$2:B$6)</f>
+        <v>0.32003720161206983</v>
+      </c>
+      <c r="D3" s="19">
+        <v>33.5</v>
+      </c>
+      <c r="E3" s="18">
+        <f t="shared" si="0"/>
+        <v>0.28341793570219964</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="14">
+        <v>12037</v>
+      </c>
+      <c r="C4" s="15">
+        <f t="shared" si="0"/>
+        <v>0.13820858163112995</v>
+      </c>
+      <c r="D4" s="19">
+        <v>12.7</v>
+      </c>
+      <c r="E4" s="18">
+        <f t="shared" si="0"/>
+        <v>0.10744500846023688</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="14">
+        <v>12831</v>
+      </c>
+      <c r="C5" s="15">
+        <f t="shared" si="0"/>
+        <v>0.14732527298405154</v>
+      </c>
+      <c r="D5" s="19">
+        <v>22.8</v>
+      </c>
+      <c r="E5" s="18">
+        <f t="shared" si="0"/>
+        <v>0.19289340101522842</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2454</v>
+      </c>
+      <c r="C6" s="15">
+        <f t="shared" si="0"/>
+        <v>2.8176776549206022E-2</v>
+      </c>
+      <c r="D6" s="19">
+        <v>6.7</v>
+      </c>
+      <c r="E6" s="18">
+        <f t="shared" si="0"/>
+        <v>5.6683587140439931E-2</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>